<commit_message>
started redoing Ath1 analysis
</commit_message>
<xml_diff>
--- a/Sly1/output/allDEGs_notes.xlsx
+++ b/Sly1/output/allDEGs_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levla\github\Ath_RNAseq\Sly1\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93ED1BCC-DC24-4D5E-8672-70D4C3FED7AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F626DF-0CDC-4055-9754-495394E19159}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{9F797F00-55C7-4E9E-A9C2-FF1B41EC6504}"/>
   </bookViews>
@@ -1064,9 +1064,6 @@
     </r>
   </si>
   <si>
-    <t>hexosyltransferase activity; coumaric acid hexoside enzyme (Alseekh 2015); was upregulated through ETI and PTI (immunity) by bacterial pathogen (Shi 2020)</t>
-  </si>
-  <si>
     <t>enzyme in flavonoid pathway (Sacco, 2019)</t>
   </si>
   <si>
@@ -1095,6 +1092,9 @@
   </si>
   <si>
     <t>ethylene response factor (ERF)</t>
+  </si>
+  <si>
+    <t>hexosyltransferase activity; coumaric acid hexoside enzyme (Alseekh 2015); was upregulated through ETI and PTI (immunity) by bacterial pathogen (Shi 2020), flavonoid metabolism</t>
   </si>
 </sst>
 </file>
@@ -1183,20 +1183,6 @@
   <dxfs count="20">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1233,6 +1219,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1316,24 +1316,24 @@
   <tableColumns count="18">
     <tableColumn id="3" xr3:uid="{BED748BC-54B1-4766-B83E-E74BED971703}" uniqueName="3" name="original_genename" queryTableFieldId="3" dataDxfId="17"/>
     <tableColumn id="10" xr3:uid="{7DB71AC2-2E83-42E9-8053-59AE3D4447DC}" uniqueName="10" name="gene" queryTableFieldId="10" dataDxfId="16"/>
-    <tableColumn id="1" xr3:uid="{EA5A1A0D-6720-49AD-8AD6-1DB9EDE8F562}" uniqueName="1" name="Column1" queryTableFieldId="27" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{EA5A1A0D-6720-49AD-8AD6-1DB9EDE8F562}" uniqueName="1" name="Column1" queryTableFieldId="27" dataDxfId="15">
       <calculatedColumnFormula>LEFT(allDEGs[[#This Row],[gene]], 14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CD446CDC-8B6A-44B7-88D8-3B278555E513}" uniqueName="5" name="log2FoldChange" queryTableFieldId="5" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{E54E6C54-CE9C-4E5A-A054-E0709BBE14A9}" uniqueName="9" name="padj" queryTableFieldId="9" dataDxfId="14"/>
-    <tableColumn id="22" xr3:uid="{5D021FCD-062E-40D5-B90C-935BD0EAFE4D}" uniqueName="22" name="notes" queryTableFieldId="26" dataDxfId="0"/>
-    <tableColumn id="20" xr3:uid="{BBF3D08D-DA79-49E7-A5F1-B9EEAF290FBF}" uniqueName="20" name="compartment" queryTableFieldId="20" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{BAA08207-DD6F-40C4-AE9A-42128D33F287}" uniqueName="4" name="baseMean" queryTableFieldId="4" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{350BE5A0-3612-47AA-95C5-C54BE6D87E65}" uniqueName="6" name="lfcSE" queryTableFieldId="6" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{76F97CA2-C7F4-4A36-8370-993F05806636}" uniqueName="7" name="stat" queryTableFieldId="7" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{1D31A347-D394-40E8-9F97-FB2739DCB918}" uniqueName="8" name="pvalue" queryTableFieldId="8" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{18E4DAC0-A867-4023-B3E4-2203A8B6EDCA}" uniqueName="11" name="description_ITAG4.0" queryTableFieldId="11" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{7482856F-2D7B-47BF-9942-3BD2B38A56DB}" uniqueName="12" name="goterm" queryTableFieldId="12" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{54F65C9B-A766-43C7-9E8C-5F6291EF8B98}" uniqueName="15" name="description_ITAG3.0" queryTableFieldId="15" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{0F37F5CD-6042-4F5E-9537-A0872CD01F18}" uniqueName="16" name="athaliana_eg_homolog_ensembl_gene" queryTableFieldId="16" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{CD446CDC-8B6A-44B7-88D8-3B278555E513}" uniqueName="5" name="log2FoldChange" queryTableFieldId="5" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{E54E6C54-CE9C-4E5A-A054-E0709BBE14A9}" uniqueName="9" name="padj" queryTableFieldId="9" dataDxfId="13"/>
+    <tableColumn id="22" xr3:uid="{5D021FCD-062E-40D5-B90C-935BD0EAFE4D}" uniqueName="22" name="notes" queryTableFieldId="26" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{BBF3D08D-DA79-49E7-A5F1-B9EEAF290FBF}" uniqueName="20" name="compartment" queryTableFieldId="20" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{BAA08207-DD6F-40C4-AE9A-42128D33F287}" uniqueName="4" name="baseMean" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{350BE5A0-3612-47AA-95C5-C54BE6D87E65}" uniqueName="6" name="lfcSE" queryTableFieldId="6" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{76F97CA2-C7F4-4A36-8370-993F05806636}" uniqueName="7" name="stat" queryTableFieldId="7" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{1D31A347-D394-40E8-9F97-FB2739DCB918}" uniqueName="8" name="pvalue" queryTableFieldId="8" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{18E4DAC0-A867-4023-B3E4-2203A8B6EDCA}" uniqueName="11" name="description_ITAG4.0" queryTableFieldId="11" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{7482856F-2D7B-47BF-9942-3BD2B38A56DB}" uniqueName="12" name="goterm" queryTableFieldId="12" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{54F65C9B-A766-43C7-9E8C-5F6291EF8B98}" uniqueName="15" name="description_ITAG3.0" queryTableFieldId="15" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{0F37F5CD-6042-4F5E-9537-A0872CD01F18}" uniqueName="16" name="athaliana_eg_homolog_ensembl_gene" queryTableFieldId="16" dataDxfId="3"/>
     <tableColumn id="17" xr3:uid="{87696FF7-5EC0-43B2-ACA0-73E1240E615E}" uniqueName="17" name="athaliana_eg_homolog_associated_gene_name" queryTableFieldId="17" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{1B4EDB3D-0624-4F82-8EF0-0EDD635A663E}" uniqueName="18" name="external_gene_name" queryTableFieldId="18" dataDxfId="6"/>
-    <tableColumn id="19" xr3:uid="{AB649D73-5B10-4446-805E-6AEC15B92F4D}" uniqueName="19" name="athaliana_eg_homolog_perc_id" queryTableFieldId="19" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{1B4EDB3D-0624-4F82-8EF0-0EDD635A663E}" uniqueName="18" name="external_gene_name" queryTableFieldId="18" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{AB649D73-5B10-4446-805E-6AEC15B92F4D}" uniqueName="19" name="athaliana_eg_homolog_perc_id" queryTableFieldId="19" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1639,10 +1639,10 @@
   <dimension ref="A1:V66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,7 +2236,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>116</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>2.8194310777003202E-2</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>17</v>
@@ -2366,7 +2366,7 @@
         <v>3.4575472925088398E-2</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>17</v>
@@ -2478,7 +2478,7 @@
         <v>1.0750518523757101E-2</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>17</v>
@@ -2590,7 +2590,7 @@
         <v>2.4490000497539001E-2</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>17</v>
@@ -2702,7 +2702,7 @@
         <v>4.6524492035124099E-2</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>136</v>
@@ -4413,7 +4413,7 @@
         <v>1.0750518523757101E-2</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>17</v>
@@ -4635,7 +4635,7 @@
         <v>3.89348032603445E-2</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>17</v>
@@ -4692,7 +4692,7 @@
         <v>4.5354216531318103E-3</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>17</v>
@@ -4914,7 +4914,7 @@
         <v>4.8404413426576497E-3</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>136</v>
@@ -5246,7 +5246,7 @@
         <v>3.5268879012867897E-2</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>136</v>
@@ -5303,7 +5303,7 @@
         <v>7.5866918834588898E-3</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>136</v>

</xml_diff>